<commit_message>
Update date the estimation of error, mx and bootstrap
</commit_message>
<xml_diff>
--- a/Exp1/Experiment record.xlsx
+++ b/Exp1/Experiment record.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HKU\Research\Stephen\STAT3799\Deliverable\Exp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A141AB2A-C399-4ED2-8D4B-2677C738D300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E1817F-A251-407F-98A0-B06BD03BFF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14500" yWindow="3000" windowWidth="9200" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Time</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,10 +63,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>hy_stat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>10/19</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -84,6 +80,18 @@
   </si>
   <si>
     <t>gci</t>
+  </si>
+  <si>
+    <t>hy_stat(coverage)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hy_stat(mse)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hy_stat(error)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -106,12 +114,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -126,10 +140,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -423,9 +441,11 @@
     <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.9140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -451,21 +471,27 @@
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44515</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2">
         <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>0.3</v>
@@ -483,7 +509,8 @@
         <v>0.47099999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="3"/>
       <c r="C3">
         <v>64</v>
       </c>
@@ -503,7 +530,8 @@
         <v>0.3024</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="3"/>
       <c r="C4">
         <v>128</v>
       </c>
@@ -523,15 +551,15 @@
         <v>0.73950000000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="3">
         <v>2</v>
       </c>
       <c r="C5">
         <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5">
         <v>0.2</v>
@@ -549,7 +577,8 @@
         <v>0.35297669999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
       <c r="C6">
         <v>64</v>
       </c>
@@ -569,7 +598,8 @@
         <v>0.1236874</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
       <c r="C7">
         <v>128</v>
       </c>
@@ -588,6 +618,90 @@
       <c r="I7">
         <v>0.80807899999999999</v>
       </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>32</v>
+      </c>
+      <c r="E8">
+        <v>0.2</v>
+      </c>
+      <c r="F8">
+        <v>1.761406</v>
+      </c>
+      <c r="G8">
+        <v>0.3</v>
+      </c>
+      <c r="H8">
+        <v>0.9</v>
+      </c>
+      <c r="I8">
+        <v>1.6191660000000001</v>
+      </c>
+      <c r="J8">
+        <v>0.85</v>
+      </c>
+      <c r="K8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>64</v>
+      </c>
+      <c r="E9">
+        <v>0.2</v>
+      </c>
+      <c r="F9">
+        <v>0.94569910000000001</v>
+      </c>
+      <c r="G9">
+        <v>0.3</v>
+      </c>
+      <c r="H9">
+        <v>0.5</v>
+      </c>
+      <c r="I9">
+        <v>0.67454749999999997</v>
+      </c>
+      <c r="J9">
+        <v>0.87</v>
+      </c>
+      <c r="K9">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>128</v>
+      </c>
+      <c r="E10">
+        <v>0.2</v>
+      </c>
+      <c r="F10">
+        <v>0.42375800000000002</v>
+      </c>
+      <c r="G10">
+        <v>0.2</v>
+      </c>
+      <c r="H10">
+        <v>0.9</v>
+      </c>
+      <c r="I10">
+        <v>0.38481460000000001</v>
+      </c>
+      <c r="J10">
+        <v>0.91</v>
+      </c>
+      <c r="K10">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F13" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -621,22 +735,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
       <c r="I1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>